<commit_message>
task 3, task 4, task 12, task 27 to task 30
</commit_message>
<xml_diff>
--- a/SourceCode/2024/Basics-April2024/hasini/task 12/excelfile.xlsx
+++ b/SourceCode/2024/Basics-April2024/hasini/task 12/excelfile.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasin\OneDrive\Desktop\git hub\RPA-Developer-in-30-Days\SourceCode\2024\Basics-April2024\hasini\task 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1CFA10-D6A1-4E64-9FFB-67FC2E03E431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5776D071-9D54-4094-8E78-C29225717ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3432" yWindow="1812" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3084" yWindow="1464" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,36 +26,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
-    <t>name</t>
+    <t>uipath</t>
   </si>
   <si>
-    <t>abc</t>
+    <t>hasini</t>
   </si>
   <si>
-    <t>dfg</t>
+    <t>akira</t>
   </si>
   <si>
-    <t>hgd</t>
-  </si>
-  <si>
-    <t>kjd</t>
-  </si>
-  <si>
-    <t>place</t>
-  </si>
-  <si>
-    <t>jhgf</t>
-  </si>
-  <si>
-    <t>iyg</t>
-  </si>
-  <si>
-    <t>icy</t>
-  </si>
-  <si>
-    <t>Sheet1</t>
+    <t>nandan</t>
   </si>
 </sst>
 </file>
@@ -372,71 +354,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15A6ACF-6DC7-434E-9858-36C137FC87FF}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883F47F9-486F-413E-B226-F61E9ADD3CE2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>